<commit_message>
UPDATE: Se agrega validación de numero exterior y enlace con catalogo
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaPadron.xlsx
+++ b/public/archivos/PlantillaPadron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C83CC47-A60A-3145-A98E-F28BD398779F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A959FD6-0B66-0D49-B24B-221CC7B34ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>Remesa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Orden</t>
   </si>
@@ -164,14 +161,20 @@
     <t>Apellido_2 del menor*</t>
   </si>
   <si>
-    <t>Codigo Archivo</t>
+    <t>Distrito</t>
+  </si>
+  <si>
+    <t>Número de Polígono *</t>
+  </si>
+  <si>
+    <t>Número de sección *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,8 +203,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,28 +267,19 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -290,63 +298,64 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="1" xr:uid="{327B1967-ADA6-1342-950C-C6E15E529E7B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,141 +667,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:43" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="78" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AG1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AM1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AN1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AO1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AR1" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="AQ1" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: Se agrega template para solicitud
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaPadron.xlsx
+++ b/public/archivos/PlantillaPadron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A959FD6-0B66-0D49-B24B-221CC7B34ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9915AA-703D-F440-AEF3-A5E0909DEDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,138 +36,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
-  <si>
-    <t>Orden</t>
-  </si>
-  <si>
-    <t>Orden x mpio *</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Región</t>
-  </si>
-  <si>
-    <t>Nombres *</t>
-  </si>
-  <si>
-    <t>Apellido_1 *</t>
-  </si>
-  <si>
-    <t>Apellido_2 *</t>
-  </si>
-  <si>
-    <t>Fecha_Nac</t>
-  </si>
-  <si>
-    <t>Sexo</t>
-  </si>
-  <si>
-    <t>Edo_Nac</t>
-  </si>
-  <si>
-    <t>CURP *</t>
-  </si>
-  <si>
-    <t>Validador</t>
-  </si>
-  <si>
-    <t>Municipio *</t>
-  </si>
-  <si>
-    <t>Num_Loc</t>
-  </si>
-  <si>
-    <t>Localidad *</t>
-  </si>
-  <si>
-    <t>Colonia *</t>
-  </si>
-  <si>
-    <t>Calle *</t>
-  </si>
-  <si>
-    <t>Num_Ext *</t>
-  </si>
-  <si>
-    <t>Num_Int</t>
-  </si>
-  <si>
     <t>CP</t>
   </si>
   <si>
-    <t>Tel_Casa</t>
-  </si>
-  <si>
-    <t>Tel_Cel *</t>
-  </si>
-  <si>
-    <t>Tel_Recados</t>
-  </si>
-  <si>
-    <t>AÑO DE VIGENCIA DE INE *</t>
-  </si>
-  <si>
-    <t>FOLIO TARJETA GTO CONTIGO SÍ / IMPULSO</t>
-  </si>
-  <si>
-    <t>Apoyo_Solicitado *</t>
-  </si>
-  <si>
-    <t>Vertiente *</t>
-  </si>
-  <si>
-    <t>Enlace / Origen *</t>
-  </si>
-  <si>
-    <t>Largo_CURP</t>
-  </si>
-  <si>
-    <t>Frecuencia_CURP</t>
-  </si>
-  <si>
     <t>PERIODO</t>
   </si>
   <si>
-    <t>Nombres del menor*</t>
-  </si>
-  <si>
-    <t>Apellido_1 del menor*</t>
-  </si>
-  <si>
-    <t>Fecha_Nac_menor</t>
-  </si>
-  <si>
-    <t>Sexo_del_menor</t>
-  </si>
-  <si>
-    <t>Edo_Nac_del menor</t>
-  </si>
-  <si>
-    <t>CURP_del menor*</t>
-  </si>
-  <si>
-    <t>Validador_CURP_del_menor</t>
-  </si>
-  <si>
-    <t>Largo_CURP_menor</t>
-  </si>
-  <si>
-    <t>Frecuencia_CURP_menor</t>
-  </si>
-  <si>
-    <t>Apellido_2 del menor*</t>
-  </si>
-  <si>
-    <t>Distrito</t>
-  </si>
-  <si>
-    <t>Número de Polígono *</t>
-  </si>
-  <si>
-    <t>Número de sección *</t>
+    <t>ORDEN</t>
+  </si>
+  <si>
+    <t>ORDEN_X_MPIO</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>NOMBRES</t>
+  </si>
+  <si>
+    <t>APELLIDO_1</t>
+  </si>
+  <si>
+    <t>APELLIDO_2</t>
+  </si>
+  <si>
+    <t>FECHA_NAC</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>EDO_NAC</t>
+  </si>
+  <si>
+    <t>CURP</t>
+  </si>
+  <si>
+    <t>VALIDADOR</t>
+  </si>
+  <si>
+    <t>MUNICIPIO</t>
+  </si>
+  <si>
+    <t>NUM_LOC</t>
+  </si>
+  <si>
+    <t>LOCALIDAD</t>
+  </si>
+  <si>
+    <t>COLONIA</t>
+  </si>
+  <si>
+    <t>CVE_COLONIA</t>
+  </si>
+  <si>
+    <t>CVE_INTERVENTOR</t>
+  </si>
+  <si>
+    <t>CVE_TIPO_CALLE</t>
+  </si>
+  <si>
+    <t>CALLE</t>
+  </si>
+  <si>
+    <t>NUM_EXT</t>
+  </si>
+  <si>
+    <t>NUM_INT</t>
+  </si>
+  <si>
+    <t>TEL_CASA</t>
+  </si>
+  <si>
+    <t>TEL_CEL</t>
+  </si>
+  <si>
+    <t>TEL_RECADOS</t>
+  </si>
+  <si>
+    <t>AÑO_DE_VIGENCIA_DE_INE</t>
+  </si>
+  <si>
+    <t>FOLIO_TARJETA_CONTIGO_SI</t>
+  </si>
+  <si>
+    <t>APOYO_SOLICITADO</t>
+  </si>
+  <si>
+    <t>VERTIENTE</t>
+  </si>
+  <si>
+    <t>ENLACE_ORIGEN</t>
+  </si>
+  <si>
+    <t>LARGO_CURP</t>
+  </si>
+  <si>
+    <t>FRECUENCIA_CURP</t>
+  </si>
+  <si>
+    <t>NOMBRES_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>APELLIDO_1_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>APELLIDO_2_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>FECHA_NAC_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>SEXO_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>EDO_NAC_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>CURP_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>VALIDADOR_CURP_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>LARGO_CURP_MENOR</t>
+  </si>
+  <si>
+    <t>FRECUENCIA_CURP_DEL_MENOR</t>
+  </si>
+  <si>
+    <t>ENLACE_INTERVENCION_1</t>
+  </si>
+  <si>
+    <t>ENLACE_INTERVENCION_2</t>
+  </si>
+  <si>
+    <t>ENLACE_INTERVENCION_3</t>
+  </si>
+  <si>
+    <t>FECHA_SOLICITUD</t>
+  </si>
+  <si>
+    <t>RESPONSABLE_DE_LA_ENTREGA</t>
   </si>
 </sst>
 </file>
@@ -317,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -345,9 +360,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -667,144 +679,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A1:AR1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:44" ht="78" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="32" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="X1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="11" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="AR1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>39</v>
+      <c r="AS1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Cambios en formato de plantilla de carga y descarga de padrón
</commit_message>
<xml_diff>
--- a/public/archivos/PlantillaPadron.xlsx
+++ b/public/archivos/PlantillaPadron.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9915AA-703D-F440-AEF3-A5E0909DEDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8415082-178D-434D-8C7C-6C3F505CDE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{ED99B135-9311-0D4E-B87E-40D4C46CC0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -183,13 +183,19 @@
   </si>
   <si>
     <t>RESPONSABLE_DE_LA_ENTREGA</t>
+  </si>
+  <si>
+    <t>ESTATUS_ORIGEN</t>
+  </si>
+  <si>
+    <t>VALIDACION_DATOS_DE_CONTACTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -232,8 +238,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +301,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -327,12 +346,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -362,6 +392,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -679,15 +715,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A9C34E-97D7-7B4E-8969-873A36362A97}">
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:AY1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="47" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="44" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="54.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="45" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="32" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="53.33203125" customWidth="1"/>
+    <col min="51" max="51" width="31.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="32" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="32" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,6 +919,12 @@
       </c>
       <c r="AW1" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AY1" s="11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>